<commit_message>
further daily bug fixes
</commit_message>
<xml_diff>
--- a/data_sources/FTE_facilities_and_activities.xlsx
+++ b/data_sources/FTE_facilities_and_activities.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josepauly/Desktop/New Estimations template/Python test/data_sources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josepauly/Desktop/New Estimations template/Estimations Calulator/data_sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E93FBE4-DF3D-D54E-80EA-76C907040E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0F2FD2-D8EE-F74D-A939-84C6B5067F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1140" windowWidth="27640" windowHeight="16380" xr2:uid="{E7533777-34E0-F349-991E-4993BB08CE8F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>facility_type</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Water Use</t>
+  </si>
+  <si>
+    <t>custom_rate</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,6 +447,9 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -452,7 +458,9 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>3.5930256949999998E-4</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>

</xml_diff>